<commit_message>
Add include assistant view.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>Setup Xcode, and setup TestFlight</t>
+  </si>
+  <si>
+    <t>Add Parse.com and setup the anonymous user. Set the correct device size</t>
+  </si>
+  <si>
+    <t>Add include assistant view.</t>
   </si>
 </sst>
 </file>
@@ -38,7 +44,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm\-d\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="mm\-d\-yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -78,7 +84,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,17 +416,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="157.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -443,6 +449,43 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2">
+        <v>41930</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2">
+        <v>41931</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2">
+        <v>41932</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2">
+        <v>41933</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2">
+        <v>41934</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Four touch delegates are added.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="80" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <t>Add Parse.com and setup the anonymous user. Set the correct device size</t>
   </si>
   <si>
-    <t>Add include assistant view.</t>
+    <t xml:space="preserve">Add include assistant view. Incline UIView is not good enough, looks ok. Add UITapGestureRecognizer to AssistantView </t>
   </si>
 </sst>
 </file>
@@ -46,7 +46,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\-d\-yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -58,6 +58,22 @@
       <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -78,15 +94,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,14 +439,14 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="157.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="162.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -455,23 +475,11 @@
       <c r="A3" s="2">
         <v>41930</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>41931</v>
       </c>
-      <c r="B4" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2">
@@ -482,14 +490,27 @@
       <c r="A6" s="2">
         <v>41933</v>
       </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2">
         <v>41934</v>
       </c>
+      <c r="B7" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Load data from Parse.com and display them
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>0.5+2+0.5+1.5</t>
+  </si>
+  <si>
+    <t>Load data from Parse.com and display them on the ArticlesTableViewController</t>
   </si>
 </sst>
 </file>
@@ -442,13 +445,13 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="88.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -514,6 +517,12 @@
     <row r="8" spans="1:3">
       <c r="A8" s="2">
         <v>41935</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3">

</xml_diff>

<commit_message>
Add a UI Test. Need more design details
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -42,7 +42,10 @@
     <t>0.5+2+0.5+1.5</t>
   </si>
   <si>
-    <t>Load data from Parse.com and display them on the ArticlesTableViewController</t>
+    <t>2+0.5</t>
+  </si>
+  <si>
+    <t>Load data from Parse.com and display them on the ArticlesTableViewController. Build VoiceImagesManager to handle image</t>
   </si>
 </sst>
 </file>
@@ -518,11 +521,11 @@
       <c r="A8" s="2">
         <v>41935</v>
       </c>
-      <c r="B8" s="1">
-        <v>2</v>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3">

</xml_diff>

<commit_message>
Fix a bug in TableViewCell.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Load data from Parse.com and display them on the ArticlesTableViewController. Build VoiceImagesManager to handle image</t>
+  </si>
+  <si>
+    <t>Add ArticleTableViewCell</t>
   </si>
 </sst>
 </file>
@@ -448,7 +451,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -532,6 +535,12 @@
       <c r="A9" s="2">
         <v>41936</v>
       </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2">

</xml_diff>

<commit_message>
Fix a bug in DownView.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="26080" yWindow="-2220" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Add ArticleTableViewCell</t>
+  </si>
+  <si>
+    <t>1+2</t>
+  </si>
+  <si>
+    <t>Load images into Photo Wall</t>
   </si>
 </sst>
 </file>
@@ -451,7 +457,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -535,8 +541,8 @@
       <c r="A9" s="2">
         <v>41936</v>
       </c>
-      <c r="B9" s="1">
-        <v>1</v>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
@@ -545,6 +551,12 @@
     <row r="10" spans="1:3">
       <c r="A10" s="2">
         <v>41937</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3">

</xml_diff>

<commit_message>
Add Ad and AdManager
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26080" yWindow="-2220" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,10 +54,10 @@
     <t>1+2</t>
   </si>
   <si>
-    <t>2+1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Load images into Photo Wall. Setup the backend for ads. </t>
+    <t>2+1+0.5</t>
+  </si>
+  <si>
+    <t>Load images into Photo Wall. Setup the backend for ads. Add AdsManager to handle loading from Parse.om</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Setup view and view navigation.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Load images into Photo Wall. Setup the backend for ads. Add AdsManager to handle loading from Parse.om</t>
+  </si>
+  <si>
+    <t>Setup view and view navigation</t>
   </si>
 </sst>
 </file>
@@ -460,7 +463,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -571,6 +574,12 @@
       <c r="A12" s="2">
         <v>41939</v>
       </c>
+      <c r="B12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2">

</xml_diff>

<commit_message>
Ad System TableViewCell_s are ready now.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -60,7 +60,10 @@
     <t>Load images into Photo Wall. Setup the backend for ads. Add AdsManager to handle loading from Parse.om</t>
   </si>
   <si>
-    <t>Setup view and view navigation</t>
+    <t>0.5+3</t>
+  </si>
+  <si>
+    <t>Setup view and view navigation. Ad System TableViewCell_s are ready now.</t>
   </si>
 </sst>
 </file>
@@ -463,7 +466,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -574,11 +577,11 @@
       <c r="A12" s="2">
         <v>41939</v>
       </c>
-      <c r="B12" s="1">
-        <v>0.5</v>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3">

</xml_diff>

<commit_message>
Load text paragraph into Data Manager.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -39,30 +39,15 @@
     <t>Add include assistant view. Incline UIView is not good enough, looks ok. Add UITapGestureRecognizer to AssistantView. Add four touch delegate. Add Up and down views, including setuping NewsTableViewController</t>
   </si>
   <si>
-    <t>0.5+2+0.5+1.5</t>
-  </si>
-  <si>
-    <t>2+0.5</t>
-  </si>
-  <si>
     <t>Load data from Parse.com and display them on the ArticlesTableViewController. Build VoiceImagesManager to handle image</t>
   </si>
   <si>
     <t>Add ArticleTableViewCell</t>
   </si>
   <si>
-    <t>1+2</t>
-  </si>
-  <si>
-    <t>2+1+0.5</t>
-  </si>
-  <si>
     <t>Load images into Photo Wall. Setup the backend for ads. Add AdsManager to handle loading from Parse.om</t>
   </si>
   <si>
-    <t>0.5+3</t>
-  </si>
-  <si>
     <t>Setup view and view navigation. Ad System TableViewCell_s are ready now.</t>
   </si>
   <si>
@@ -79,6 +64,9 @@
   </si>
   <si>
     <t>Found a bug in Collection view and reloved it.</t>
+  </si>
+  <si>
+    <t>Load text paragraph.</t>
   </si>
 </sst>
 </file>
@@ -494,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -559,8 +547,9 @@
       <c r="A7" s="2">
         <v>41934</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
+      <c r="B7" s="1">
+        <f>0.5+2+0.5+1.5</f>
+        <v>4.5</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -570,33 +559,36 @@
       <c r="A8" s="2">
         <v>41935</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
+      <c r="B8" s="1">
+        <f>2+0.5</f>
+        <v>2.5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2">
         <v>41936</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
+      <c r="B9" s="1">
+        <f>1+2</f>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2">
         <v>41937</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
+      <c r="B10" s="1">
+        <f>2+1+0.5</f>
+        <v>3.5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -608,11 +600,12 @@
       <c r="A12" s="2">
         <v>41939</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
+      <c r="B12" s="1">
+        <f>0.5+3</f>
+        <v>3.5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -623,7 +616,7 @@
         <v>0.5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -634,7 +627,7 @@
         <v>1.5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -645,7 +638,7 @@
         <v>0.5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -656,7 +649,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -667,7 +660,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -681,8 +674,12 @@
       <c r="A19" s="3">
         <v>41946</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3">
@@ -690,6 +687,12 @@
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" s="1">
+        <f>SUM(B2:B19)</f>
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update backend. No articleDetail class anymore.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="29580" yWindow="-2500" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Load text paragraph.</t>
+  </si>
+  <si>
+    <t>Update backend. No articleDetail class anymore.</t>
   </si>
 </sst>
 </file>
@@ -484,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -685,13 +688,17 @@
       <c r="A20" s="3">
         <v>41947</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
       <c r="B27" s="1">
-        <f>SUM(B2:B19)</f>
-        <v>28</v>
+        <f>SUM(B2:B20)</f>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reduce CPU Computation when loading GIF.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Add launch gif.</t>
+  </si>
+  <si>
+    <t>Reduce GPU computation when loading GIF.</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -727,11 +730,17 @@
       <c r="A23" s="3">
         <v>41950</v>
       </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
       <c r="B27" s="1">
-        <f>SUM(B2:B22)</f>
-        <v>30</v>
+        <f>SUM(B2:B23)</f>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update VoiceImage to StreetImage.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
     <t>Add launch gif.</t>
   </si>
   <si>
-    <t>Reduce GPU computation when loading GIF. Create VoicePFImage to handle image loading</t>
+    <t>Reduce GPU computation when loading GIF. Create VoicePFImage to handle image loading. AssistantHorizontalView works now.</t>
   </si>
 </sst>
 </file>
@@ -497,7 +497,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -731,17 +731,32 @@
         <v>41950</v>
       </c>
       <c r="B23" s="1">
-        <f>1+1</f>
-        <v>2</v>
+        <f>1+1+1</f>
+        <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3">
+        <v>41951</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="3">
+        <v>41952</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="3">
+        <v>41953</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="B27" s="1">
         <f>SUM(B2:B23)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix a bug in image wall - greatly reduce CPU.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
     <t>Reduce GPU computation when loading GIF. Create VoicePFImage to handle image loading. AssistantHorizontalView works now.</t>
   </si>
   <si>
-    <t>Update backend to store more images.</t>
+    <t>Update backend to store more images. Button on AssistantHorizontalView works now.</t>
   </si>
 </sst>
 </file>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -750,7 +750,8 @@
         <v>41951</v>
       </c>
       <c r="B24" s="1">
-        <v>1</v>
+        <f>1+3</f>
+        <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>20</v>
@@ -769,7 +770,7 @@
     <row r="42" spans="2:2">
       <c r="B42" s="1">
         <f>SUM(B2:B24)</f>
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update paragraph in the article.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Update backend to store more images. Button on AssistantHorizontalView works now.</t>
+  </si>
+  <si>
+    <t>Update cover image. Update paragraphes.</t>
   </si>
 </sst>
 </file>
@@ -503,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A30"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -761,6 +764,12 @@
       <c r="A25" s="3">
         <v>41952</v>
       </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3">
@@ -789,8 +798,8 @@
     </row>
     <row r="42" spans="2:2">
       <c r="B42" s="1">
-        <f>SUM(B2:B24)</f>
-        <v>37</v>
+        <f>SUM(B2:B25)</f>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Greatly improve the UI animation.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Update cover image. Update paragraphes.</t>
+  </si>
+  <si>
+    <t>Update UI and animation of the assistant view.</t>
   </si>
 </sst>
 </file>
@@ -507,7 +510,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -775,6 +778,12 @@
       <c r="A26" s="3">
         <v>41953</v>
       </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="3">
@@ -798,8 +807,8 @@
     </row>
     <row r="42" spans="2:2">
       <c r="B42" s="1">
-        <f>SUM(B2:B25)</f>
-        <v>39</v>
+        <f>SUM(B2:B26)</f>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Delegation chain is ready.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Update UI and animation of the assistant view.</t>
+  </si>
+  <si>
+    <t>Update street images. Setup the relation between several views.</t>
   </si>
 </sst>
 </file>
@@ -509,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -789,26 +792,82 @@
       <c r="A27" s="3">
         <v>41954</v>
       </c>
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="3">
         <v>41955</v>
       </c>
+      <c r="B28" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="3">
         <v>41956</v>
       </c>
+      <c r="B29" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="3">
         <v>41957</v>
       </c>
-    </row>
-    <row r="42" spans="2:2">
+      <c r="B30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="3">
+        <v>41958</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="3">
+        <v>41959</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="3">
+        <v>41960</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="3">
+        <v>41961</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="3">
+        <v>41962</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="3">
+        <v>41963</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="3">
+        <v>41964</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="B42" s="1">
-        <f>SUM(B2:B26)</f>
-        <v>40</v>
+        <f>SUM(B2:B32)</f>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Load multiply images on the screen.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Update street images class. Setup the relation between several views.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load multiply images on the screen. </t>
   </si>
 </sst>
 </file>
@@ -522,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -907,6 +910,12 @@
       <c r="A39" s="3">
         <v>41966</v>
       </c>
+      <c r="B39" s="1">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="3">
@@ -920,8 +929,8 @@
     </row>
     <row r="48" spans="1:3">
       <c r="B48" s="1">
-        <f>SUM(B2:B38)</f>
-        <v>42</v>
+        <f>SUM(B2:B39)</f>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update image loading method.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -99,7 +99,7 @@
     <t>Update street images class. Setup the relation between several views.</t>
   </si>
   <si>
-    <t>Load multiply images on the screen. Add progress indicator. Add swipe right animation. Update UI, and delete unused code.</t>
+    <t>Load multiply images on the screen. Add progress indicator. Add swipe right animation. Update UI, and delete unused code. Update article table loading method. It's much faster now.</t>
   </si>
 </sst>
 </file>
@@ -911,8 +911,8 @@
         <v>41966</v>
       </c>
       <c r="B39" s="1">
-        <f>2+0.5+0.5+1.5</f>
-        <v>4.5</v>
+        <f>2+0.5+0.5+1.5+1</f>
+        <v>5.5</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>26</v>
@@ -931,7 +931,7 @@
     <row r="48" spans="1:3">
       <c r="B48" s="1">
         <f>SUM(B2:B40)</f>
-        <v>46.5</v>
+        <v>47.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix a bug - SVProgressHub dismiss.
</commit_message>
<xml_diff>
--- a/Timelist.xlsx
+++ b/Timelist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Load multiply images on the screen. Add progress indicator. Add swipe right animation. Update UI, and delete unused code. Update article table loading method. It's much faster now.</t>
+  </si>
+  <si>
+    <t>Able to swipe to hide the article.</t>
   </si>
 </sst>
 </file>
@@ -525,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -922,16 +925,37 @@
       <c r="A40" s="3">
         <v>41967</v>
       </c>
+      <c r="B40" s="1">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="3">
         <v>41968</v>
       </c>
     </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="3">
+        <v>41969</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="3">
+        <v>41970</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="3">
+        <v>41971</v>
+      </c>
+    </row>
     <row r="48" spans="1:3">
       <c r="B48" s="1">
         <f>SUM(B2:B40)</f>
-        <v>47.5</v>
+        <v>49.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>